<commit_message>
Added demo example and description
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelkolb/Dropbox/KULeuven/PhD/Meetings/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelkolb/Documents/PhD/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sum, Average, ..." sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Mapping or In Set" sheetId="7" r:id="rId6"/>
     <sheet name="Conditional Sum..." sheetId="8" r:id="rId7"/>
     <sheet name="Previous (fold)" sheetId="9" r:id="rId8"/>
+    <sheet name="Combined" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="38">
   <si>
     <t>Salesperson</t>
   </si>
@@ -151,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +181,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,12 +209,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +708,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -695,7 +719,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,7 +783,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -768,7 +794,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,7 +848,9 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -831,7 +859,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D1" sqref="D1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,7 +966,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -947,7 +977,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C1" sqref="C1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,9 +1006,8 @@
       <c r="B2" s="1">
         <v>1514</v>
       </c>
-      <c r="C2" t="str">
-        <f>LOOKUP(B2/$B$7,$E$2:$E$4,$F$2:$F$4)</f>
-        <v>Great</v>
+      <c r="C2" t="s">
+        <v>26</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -994,9 +1023,8 @@
       <c r="B3" s="1">
         <v>1551</v>
       </c>
-      <c r="C3" t="str">
-        <f>LOOKUP(B3/$B$7,$E$2:$E$4,$F$2:$F$4)</f>
-        <v>Great</v>
+      <c r="C3" t="s">
+        <v>26</v>
       </c>
       <c r="E3" s="4">
         <v>0.8</v>
@@ -1012,9 +1040,8 @@
       <c r="B4" s="1">
         <v>691</v>
       </c>
-      <c r="C4" t="str">
-        <f>LOOKUP(B4/$B$7,$E$2:$E$4,$F$2:$F$4)</f>
-        <v>Low</v>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="4">
         <v>1.2</v>
@@ -1030,9 +1057,8 @@
       <c r="B5" s="1">
         <v>392</v>
       </c>
-      <c r="C5" t="str">
-        <f>LOOKUP(B5/$B$7,$E$2:$E$4,$F$2:$F$4)</f>
-        <v>Low</v>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1044,16 +1070,18 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1157,17 +1185,27 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B1" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,7 +1217,7 @@
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1195,8 +1233,10 @@
       <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1213,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1230,7 +1270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -1272,7 +1312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>1</v>
       </c>
@@ -1296,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>3</v>
       </c>
@@ -1313,7 +1353,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1322,7 +1364,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,6 +1450,642 @@
       <c r="C12" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>353</v>
+      </c>
+      <c r="D2" s="7">
+        <v>378</v>
+      </c>
+      <c r="E2" s="7">
+        <v>396</v>
+      </c>
+      <c r="F2" s="7">
+        <v>387</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1514</v>
+      </c>
+      <c r="H2" s="6">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>370</v>
+      </c>
+      <c r="D3" s="7">
+        <v>408</v>
+      </c>
+      <c r="E3" s="7">
+        <v>387</v>
+      </c>
+      <c r="F3" s="7">
+        <v>386</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1551</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6">
+        <v>29</v>
+      </c>
+      <c r="K3" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>175</v>
+      </c>
+      <c r="D4" s="7">
+        <v>146</v>
+      </c>
+      <c r="E4" s="7">
+        <v>167</v>
+      </c>
+      <c r="F4" s="7">
+        <v>203</v>
+      </c>
+      <c r="G4" s="7">
+        <v>691</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="6">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
+        <v>93</v>
+      </c>
+      <c r="D5" s="7">
+        <v>98</v>
+      </c>
+      <c r="E5" s="7">
+        <v>96</v>
+      </c>
+      <c r="F5" s="7">
+        <v>105</v>
+      </c>
+      <c r="G5" s="7">
+        <v>392</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="6">
+        <v>17</v>
+      </c>
+      <c r="K5" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8">
+        <v>991</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1030</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1046</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1081</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4148</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8">
+        <v>247.75</v>
+      </c>
+      <c r="D8" s="6">
+        <v>257.5</v>
+      </c>
+      <c r="E8" s="8">
+        <v>261.5</v>
+      </c>
+      <c r="F8" s="8">
+        <v>270.25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1037</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8">
+        <v>370</v>
+      </c>
+      <c r="D9" s="8">
+        <v>408</v>
+      </c>
+      <c r="E9" s="8">
+        <v>396</v>
+      </c>
+      <c r="F9" s="8">
+        <v>387</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1551</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8">
+        <v>93</v>
+      </c>
+      <c r="D10" s="8">
+        <v>98</v>
+      </c>
+      <c r="E10" s="8">
+        <v>96</v>
+      </c>
+      <c r="F10" s="8">
+        <v>105</v>
+      </c>
+      <c r="G10" s="8">
+        <v>392</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>10</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="6">
+        <v>8</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <v>9</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="6">
+        <v>15</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="6">
+        <v>8</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="8">
+        <v>991</v>
+      </c>
+      <c r="D20" s="8">
+        <v>212</v>
+      </c>
+      <c r="E20" s="8">
+        <v>779</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>20</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1030</v>
+      </c>
+      <c r="D21" s="8">
+        <v>710</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1099</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1046</v>
+      </c>
+      <c r="D22" s="8">
+        <v>137</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2008</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="6">
+        <v>19</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1081</v>
+      </c>
+      <c r="D23" s="8">
+        <v>240</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2849</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>